<commit_message>
Wednesday 8 May 2024
</commit_message>
<xml_diff>
--- a/Price Comparison.xlsx
+++ b/Price Comparison.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fs1\StudentHome$\Students\21308\Documents\Year 12\CSC2\AS91896 &amp; AS91897\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fs1\StudentHome$\Students\21308\Documents\Year 12\CSC2 - Assessment\AS91896 &amp; AS91897\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B1DED35-2761-4975-8214-E28490A35034}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{623D9E3F-DCBE-4684-A2ED-76D676629C53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{F92DFA60-38E8-49E4-AA3F-02FDAB998F42}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +520,7 @@
         <v>185</v>
       </c>
       <c r="C6">
-        <f>B6/1000</f>
+        <f t="shared" ref="C6:C11" si="0">B6/1000</f>
         <v>0.185</v>
       </c>
       <c r="D6" s="3">
@@ -539,11 +539,15 @@
         <v>250</v>
       </c>
       <c r="C7">
-        <f>B7/1000</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="D7" s="3">
         <v>2.5</v>
+      </c>
+      <c r="E7" s="3">
+        <f>D7/C7</f>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -554,11 +558,15 @@
         <v>190</v>
       </c>
       <c r="C8">
-        <f>B8/1000</f>
+        <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
       <c r="D8" s="3">
         <v>3.3</v>
+      </c>
+      <c r="E8" s="3">
+        <f>D8/C8</f>
+        <v>17.368421052631579</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -569,11 +577,15 @@
         <v>250</v>
       </c>
       <c r="C9">
-        <f>B9/1000</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="D9" s="3">
         <v>3.99</v>
+      </c>
+      <c r="E9" s="3">
+        <f>D9/C9</f>
+        <v>15.96</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -584,11 +596,15 @@
         <v>170</v>
       </c>
       <c r="C10">
-        <f>B10/1000</f>
+        <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
       <c r="D10" s="3">
         <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <f>D10/C10</f>
+        <v>11.76470588235294</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,11 +615,15 @@
         <v>100</v>
       </c>
       <c r="C11">
-        <f>B11/1000</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="D11" s="3">
         <v>1.65</v>
+      </c>
+      <c r="E11" s="3">
+        <f>D11/C11</f>
+        <v>16.499999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>